<commit_message>
Added Accellerometer and sparkfun sensor library
</commit_message>
<xml_diff>
--- a/Bill of materials.xlsx
+++ b/Bill of materials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avuon\OneDrive\Desktop\github\EE-109K---PCB-Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fred8\OneDrive\Desktop\UT\Semester 2\EE 109k - First Year Design Experience\Bike Alarm Repo\EE-109K---PCB-Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450D0500-5639-4FFC-8007-89E26E76F624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F6926A-54E4-4B93-90BA-3A5FEA18CAFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7776" yWindow="1752" windowWidth="12264" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>GPS module(NEO-6M)</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>https://www.amazon.com/Passive-Buzzer-Arduino-3-3V-5V-Interface/dp/B07KNV8KVJ</t>
+  </si>
+  <si>
+    <t>Accelerometer</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/12786</t>
   </si>
 </sst>
 </file>
@@ -369,15 +375,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:C4"/>
+  <dimension ref="A3:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="19.89453125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -388,7 +397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -397,11 +406,23 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{A8B549FC-7A13-4BB4-872B-4255DEFFDF8A}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{E68677A9-08BF-4CA3-A387-1CE739DF6245}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed Schematic, no text module
</commit_message>
<xml_diff>
--- a/Bill of materials.xlsx
+++ b/Bill of materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fred8\OneDrive\Desktop\UT\Semester 2\EE 109k - First Year Design Experience\Bike Alarm Repo\EE-109K---PCB-Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F6926A-54E4-4B93-90BA-3A5FEA18CAFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10DD250-78BD-4465-B7C1-416902551E37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,7 +378,7 @@
   <dimension ref="A3:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>